<commit_message>
Updated images and reordered variants.
</commit_message>
<xml_diff>
--- a/SSoT/WorkingDir/MorseCodeSDK.xlsx
+++ b/SSoT/WorkingDir/MorseCodeSDK.xlsx
@@ -21,6 +21,18 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>Continental</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
     <t>RelativeLength</t>
   </si>
   <si>
@@ -33,25 +45,16 @@
     <t>Binary</t>
   </si>
   <si>
-    <t>Creator</t>
+    <t>Dot</t>
   </si>
   <si>
-    <t>American</t>
-  </si>
-  <si>
-    <t>Continental</t>
-  </si>
-  <si>
-    <t>International</t>
-  </si>
-  <si>
-    <t>Dot</t>
+    <t>_</t>
   </si>
   <si>
     <t>short mark or dot (▄▄▄▄)</t>
   </si>
   <si>
-    <t>_</t>
+    <t>-x-x-x-x-</t>
   </si>
   <si>
     <t>.</t>
@@ -67,9 +70,6 @@
   </si>
   <si>
     <t>LongDash</t>
-  </si>
-  <si>
-    <t>-x-x-x-x-</t>
   </si>
   <si>
     <t>"long dash" (▄▄▄▄▄▄▄, the letter L)</t>
@@ -90,28 +90,28 @@
     <t>.x.x.x-x.</t>
   </si>
   <si>
+    <t>.x.x.x-x-</t>
+  </si>
+  <si>
+    <t>International morse code has been adopted by most of the rest of the world</t>
+  </si>
+  <si>
+    <t>ITU</t>
+  </si>
+  <si>
     <t>American or Railroad Morsecode was designed b y morse</t>
   </si>
   <si>
     <t>Morse</t>
   </si>
   <si>
-    <t>.x.x.x-x-</t>
-  </si>
-  <si>
     <t>The Gerke code was adopted as a standard for transmission over cables by the Austro-German Telegraph Union, and this was called Continental Code</t>
-  </si>
-  <si>
-    <t>Gerke</t>
   </si>
   <si>
     <t>.x.x.x.x-</t>
   </si>
   <si>
-    <t>International morse code has been adopted by most of the rest of the world</t>
-  </si>
-  <si>
-    <t>ITU</t>
+    <t>Gerke</t>
   </si>
   <si>
     <t>-x-x-</t>
@@ -123,10 +123,10 @@
     <t>.x.x.x.x.x.</t>
   </si>
   <si>
-    <t>--</t>
+    <t>-x.x.x.x.</t>
   </si>
   <si>
-    <t>-x.x.x.x.</t>
+    <t>--</t>
   </si>
   <si>
     <t>ExtraLongDash</t>
@@ -138,22 +138,31 @@
     <t>---</t>
   </si>
   <si>
+    <t>ICG</t>
+  </si>
+  <si>
     <t>-x-x.x.</t>
   </si>
   <si>
-    <t>ICG</t>
+    <t>intra-character gap (standard gap between the dots and dashes in a character)</t>
   </si>
   <si>
     <t>-x-x.x.x.</t>
   </si>
   <si>
-    <t>intra-character gap (standard gap between the dots and dashes in a character)</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
+    <t>-x-x-x.x.</t>
+  </si>
+  <si>
+    <t>-x.x.x-</t>
+  </si>
+  <si>
     <t>LongICG</t>
+  </si>
+  <si>
+    <t>-x-x-x-x.</t>
   </si>
   <si>
     <t>long intra-character gap (longer internal gap used in C, O, R, Y, Z and &amp;)</t>
@@ -162,7 +171,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>-x-x-x.x.</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>.x-</t>
   </si>
   <si>
     <t>ShortGap</t>
@@ -174,13 +186,13 @@
     <t>l</t>
   </si>
   <si>
-    <t>-x.x.x-</t>
-  </si>
-  <si>
-    <t>-x-x-x-x.</t>
+    <t>B</t>
   </si>
   <si>
     <t>MediumGap</t>
+  </si>
+  <si>
+    <t>-x.x.x.</t>
   </si>
   <si>
     <t>medium gap (between words)</t>
@@ -189,25 +201,13 @@
     <t>w</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>LongGap</t>
-  </si>
-  <si>
-    <t>.x-</t>
   </si>
   <si>
     <t>long gap (between sentences)</t>
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>-x.x.x.</t>
   </si>
   <si>
     <t>C</t>
@@ -384,12 +384,12 @@
       <sz val="10.0"/>
     </font>
     <font>
+      <sz val="10.0"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF222222"/>
       <name val="Sans-serif"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
     </font>
     <font/>
   </fonts>
@@ -423,30 +423,30 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -482,14 +482,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -516,35 +516,35 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
+      <c r="A2" s="9" t="s">
+        <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>8</v>
+      <c r="A3" s="9" t="s">
+        <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
+      <c r="A4" s="9" t="s">
+        <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>31</v>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -569,24 +569,265 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f>"="</f>
+        <v>=</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="9" t="str">
+        <f>" "</f>
+        <v> </v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" ht="10.5" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="9" t="str">
+        <f>"  "</f>
+        <v>  </v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="9" t="str">
+        <f>"   "</f>
+        <v>   </v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="9" t="str">
+        <f>"    "</f>
+        <v>    </v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="9" t="str">
+        <f>"     "</f>
+        <v>     </v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.0"/>
+    <col customWidth="1" min="2" max="2" width="9.57"/>
+    <col customWidth="1" min="3" max="3" width="10.43"/>
+    <col customWidth="1" min="4" max="4" width="11.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -607,260 +848,19 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>10</v>
+      <c r="A2" s="6">
+        <v>0.0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8">
-        <v>1.0</v>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f>"="</f>
-        <v>=</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="8" t="str">
-        <f>" "</f>
-        <v> </v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" ht="10.5" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="8" t="str">
-        <f>"  "</f>
-        <v>  </v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="8" t="str">
-        <f>"   "</f>
-        <v>   </v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="8" t="str">
-        <f>"    "</f>
-        <v>    </v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="8" t="str">
-        <f>"     "</f>
-        <v>     </v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="6.0"/>
-    <col customWidth="1" min="2" max="2" width="9.57"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="11.14"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -886,16 +886,16 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>1.0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="10"/>
@@ -922,16 +922,16 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>2.0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="10"/>
@@ -958,17 +958,17 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>3.0</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>27</v>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -994,17 +994,17 @@
       <c r="Z5" s="10"/>
     </row>
     <row r="6">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>4.0</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>30</v>
+      <c r="B6" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>30</v>
+      <c r="C6" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>30</v>
+      <c r="D6" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -1030,16 +1030,16 @@
       <c r="Z6" s="10"/>
     </row>
     <row r="7">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>5.0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="10"/>
@@ -1066,17 +1066,17 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>6.0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>37</v>
+      <c r="D8" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -1102,17 +1102,17 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>7.0</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>41</v>
+      <c r="B9" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>41</v>
+      <c r="C9" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>43</v>
+      <c r="D9" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -1138,17 +1138,17 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>8.0</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>37</v>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>49</v>
+      <c r="D10" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -1174,17 +1174,17 @@
       <c r="Z10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>9.0</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>53</v>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>53</v>
+      <c r="C11" s="8" t="s">
+        <v>47</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>54</v>
+      <c r="D11" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1210,17 +1210,17 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>58</v>
+      <c r="A12" s="6" t="s">
+        <v>52</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>60</v>
+      <c r="B12" s="8" t="s">
+        <v>53</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>60</v>
+      <c r="C12" s="8" t="s">
+        <v>53</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>60</v>
+      <c r="D12" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1246,17 +1246,17 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>63</v>
+      <c r="A13" s="6" t="s">
+        <v>57</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>64</v>
+      <c r="B13" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>64</v>
+      <c r="C13" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>64</v>
+      <c r="D13" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1282,16 +1282,16 @@
       <c r="Z13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="10"/>
@@ -1318,16 +1318,16 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>69</v>
       </c>
       <c r="E15" s="10"/>
@@ -1354,17 +1354,17 @@
       <c r="Z15" s="10"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>13</v>
+      <c r="B16" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>13</v>
+      <c r="C16" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>13</v>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1390,16 +1390,16 @@
       <c r="Z16" s="10"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>73</v>
       </c>
       <c r="E17" s="10"/>
@@ -1426,16 +1426,16 @@
       <c r="Z17" s="10"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E18" s="10"/>
@@ -1462,16 +1462,16 @@
       <c r="Z18" s="10"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>78</v>
       </c>
       <c r="E19" s="10"/>
@@ -1498,16 +1498,16 @@
       <c r="Z19" s="10"/>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="10"/>
@@ -1534,16 +1534,16 @@
       <c r="Z20" s="10"/>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>82</v>
       </c>
       <c r="E21" s="10"/>
@@ -1570,16 +1570,16 @@
       <c r="Z21" s="10"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="10"/>
@@ -1606,17 +1606,17 @@
       <c r="Z22" s="10"/>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B23" s="10" t="str">
         <f>"="</f>
         <v>=</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>86</v>
       </c>
       <c r="E23" s="10"/>
@@ -1643,16 +1643,16 @@
       <c r="Z23" s="10"/>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>88</v>
       </c>
       <c r="E24" s="10"/>
@@ -1679,16 +1679,16 @@
       <c r="Z24" s="10"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>90</v>
       </c>
       <c r="E25" s="10"/>
@@ -1715,16 +1715,16 @@
       <c r="Z25" s="10"/>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="10"/>
@@ -1751,16 +1751,16 @@
       <c r="Z26" s="10"/>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="10"/>
@@ -1787,16 +1787,16 @@
       <c r="Z27" s="10"/>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E28" s="10"/>
@@ -1823,16 +1823,16 @@
       <c r="Z28" s="10"/>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E29" s="10"/>
@@ -1859,16 +1859,16 @@
       <c r="Z29" s="10"/>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>100</v>
       </c>
       <c r="E30" s="10"/>
@@ -1895,17 +1895,17 @@
       <c r="Z30" s="10"/>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>16</v>
+      <c r="B31" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>16</v>
+      <c r="C31" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>16</v>
+      <c r="D31" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1931,16 +1931,16 @@
       <c r="Z31" s="10"/>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="10"/>
@@ -1967,16 +1967,16 @@
       <c r="Z32" s="10"/>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>105</v>
       </c>
       <c r="E33" s="10"/>
@@ -2003,16 +2003,16 @@
       <c r="Z33" s="10"/>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E34" s="10"/>
@@ -2039,17 +2039,17 @@
       <c r="Z34" s="10"/>
     </row>
     <row r="35">
-      <c r="A35" s="7" t="s">
-        <v>48</v>
+      <c r="A35" s="6" t="s">
+        <v>51</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>53</v>
+      <c r="D35" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -2075,16 +2075,16 @@
       <c r="Z35" s="10"/>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>43</v>
+      <c r="C36" s="8" t="s">
+        <v>44</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>111</v>
       </c>
       <c r="E36" s="10"/>
@@ -2111,17 +2111,17 @@
       <c r="Z36" s="10"/>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>41</v>
+      <c r="D37" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2147,10 +2147,10 @@
       <c r="Z37" s="10"/>
     </row>
     <row r="38">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C38" s="10"/>

</xml_diff>

<commit_message>
Example of what happens when removing a variant.
</commit_message>
<xml_diff>
--- a/SSoT/WorkingDir/MorseCodeSDK.xlsx
+++ b/SSoT/WorkingDir/MorseCodeSDK.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -33,16 +33,13 @@
     <t>Binary</t>
   </si>
   <si>
+    <t>Dot</t>
+  </si>
+  <si>
     <t>Creator</t>
   </si>
   <si>
-    <t>Dot</t>
-  </si>
-  <si>
     <t>short mark or dot (▄▄▄▄)</t>
-  </si>
-  <si>
-    <t>International</t>
   </si>
   <si>
     <t>American</t>
@@ -51,16 +48,13 @@
     <t>Continental</t>
   </si>
   <si>
+    <t>International</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
-    <t>International morse code has been adopted by most of the rest of the world</t>
-  </si>
-  <si>
     <t>Dash</t>
-  </si>
-  <si>
-    <t>ITU</t>
   </si>
   <si>
     <t>longer mark or dash (▄▄▄▄▄)</t>
@@ -69,25 +63,10 @@
     <t>-</t>
   </si>
   <si>
-    <t>American or Railroad Morsecode was designed b y morse</t>
-  </si>
-  <si>
-    <t>Morse</t>
-  </si>
-  <si>
     <t>LongDash</t>
   </si>
   <si>
     <t>"long dash" (▄▄▄▄▄▄▄, the letter L)</t>
-  </si>
-  <si>
-    <t>The Gerke code was adopted as a standard for transmission over cables by the Austro-German Telegraph Union, and this was called Continental Code</t>
-  </si>
-  <si>
-    <t>Gerke</t>
-  </si>
-  <si>
-    <t>_</t>
   </si>
   <si>
     <t>--</t>
@@ -97,6 +76,9 @@
   </si>
   <si>
     <t>even longer dash (▄▄▄▄▄▄▄▄▄▄▄▄▄▄, the numeral 0)</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
   <si>
     <t>---</t>
@@ -111,13 +93,25 @@
     <t>x</t>
   </si>
   <si>
+    <t>International morse code has been adopted by most of the rest of the world</t>
+  </si>
+  <si>
+    <t>ITU</t>
+  </si>
+  <si>
     <t>LongICG</t>
+  </si>
+  <si>
+    <t>-x-x-x-x-</t>
+  </si>
+  <si>
+    <t>American or Railroad Morsecode was designed b y morse</t>
   </si>
   <si>
     <t>long intra-character gap (longer internal gap used in C, O, R, Y, Z and &amp;)</t>
   </si>
   <si>
-    <t>-x-x-x-x-</t>
+    <t>Morse</t>
   </si>
   <si>
     <t>X</t>
@@ -132,6 +126,12 @@
     <t>l</t>
   </si>
   <si>
+    <t>.x-x-x.</t>
+  </si>
+  <si>
+    <t>.x-x-x-x-</t>
+  </si>
+  <si>
     <t>MediumGap</t>
   </si>
   <si>
@@ -141,25 +141,19 @@
     <t>w</t>
   </si>
   <si>
+    <t>.x.x-x.x.</t>
+  </si>
+  <si>
+    <t>.x.x-x-x-</t>
+  </si>
+  <si>
     <t>LongGap</t>
   </si>
   <si>
     <t>long gap (between sentences)</t>
   </si>
   <si>
-    <t>.x-x-x.</t>
-  </si>
-  <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>.x-x-x-x-</t>
-  </si>
-  <si>
-    <t>.x.x-x.x.</t>
-  </si>
-  <si>
-    <t>.x.x-x-x-</t>
   </si>
   <si>
     <t>.x.x.x-x.</t>
@@ -423,11 +417,10 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -438,6 +431,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -479,71 +473,65 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>15</v>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -584,211 +572,211 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
+      <c r="A2" s="4" t="s">
+        <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>1.0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>4.0</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" s="6" t="str">
         <f>"="</f>
         <v>=</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="7" t="str">
+      <c r="E6" s="6" t="str">
         <f>" "</f>
         <v> </v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>0.0</v>
       </c>
     </row>
     <row r="7" ht="10.5" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>32</v>
+      <c r="A7" s="4" t="s">
+        <v>28</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="str">
+      <c r="E7" s="6" t="str">
         <f>"  "</f>
         <v>  </v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>0.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="7" t="str">
+      <c r="E8" s="6" t="str">
         <f>"   "</f>
         <v>   </v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>3.0</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="7" t="str">
+      <c r="E9" s="6" t="str">
         <f>"    "</f>
         <v>    </v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>0.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>42</v>
+      <c r="A10" s="4" t="s">
+        <v>44</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>4.0</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
+      <c r="D10" s="6" t="s">
+        <v>46</v>
       </c>
-      <c r="E10" s="7" t="str">
+      <c r="E10" s="6" t="str">
         <f>"     "</f>
         <v>     </v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>0.0</v>
       </c>
     </row>
@@ -811,53 +799,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="9">
         <v>0.0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -887,13 +875,13 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -923,13 +911,13 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -959,13 +947,13 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -995,13 +983,13 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -1031,13 +1019,13 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -1067,13 +1055,13 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -1103,13 +1091,13 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1139,13 +1127,13 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -1175,13 +1163,13 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1208,16 +1196,16 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1244,16 +1232,16 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -1280,16 +1268,16 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="D14" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1316,16 +1304,16 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -1352,7 +1340,7 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>12</v>
@@ -1388,16 +1376,16 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="D17" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1424,16 +1412,16 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1460,16 +1448,16 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -1496,16 +1484,16 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1532,16 +1520,16 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1568,16 +1556,16 @@
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -1604,17 +1592,17 @@
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="11" t="str">
         <f>"="</f>
         <v>=</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -1641,16 +1629,16 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -1677,16 +1665,16 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -1713,16 +1701,16 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="D26" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -1749,16 +1737,16 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -1785,16 +1773,16 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -1821,16 +1809,16 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -1857,16 +1845,16 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -1893,16 +1881,16 @@
     </row>
     <row r="31">
       <c r="A31" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -1929,16 +1917,16 @@
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
@@ -1965,16 +1953,16 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -2001,16 +1989,16 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -2037,16 +2025,16 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -2073,16 +2061,16 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2109,16 +2097,16 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>113</v>
-      </c>
       <c r="D37" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -2145,10 +2133,10 @@
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>

</xml_diff>